<commit_message>
performed preprocessing audit, reran updated lasso after fix
</commit_message>
<xml_diff>
--- a/Publication/Outputs/Tables/ST3.xlsx
+++ b/Publication/Outputs/Tables/ST3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t xml:space="preserve">Machine Learning Model</t>
   </si>
@@ -35,13 +35,13 @@
     <t xml:space="preserve">LASSO</t>
   </si>
   <si>
-    <t xml:space="preserve">0.80 [0.79–0.81]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69% [67%–71%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75% [70%–77%]</t>
+    <t xml:space="preserve">0.79 [0.57–0.95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66% [33%–100%]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74% [62%–82%]</t>
   </si>
   <si>
     <t xml:space="preserve">Simplified; Y; N</t>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">0.71 [0.48–0.96]</t>
   </si>
   <si>
-    <t xml:space="preserve">66% [33%–100%]</t>
-  </si>
-  <si>
     <t xml:space="preserve">65% [54%–77%]</t>
   </si>
   <si>
@@ -209,13 +206,7 @@
     <t xml:space="preserve">0.77 [0.57–0.94]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.80 [0.79–0.80]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4% [0%–8%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% [100%–100%]</t>
+    <t xml:space="preserve">2% [0%–20%]</t>
   </si>
   <si>
     <t xml:space="preserve">0.63 [0.44–0.87]</t>
@@ -605,7 +596,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -731,10 +722,10 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -748,13 +739,13 @@
         <v>0.29</v>
       </c>
       <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -762,19 +753,19 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>0.27</v>
       </c>
       <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -788,13 +779,13 @@
         <v>0.27</v>
       </c>
       <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -808,33 +799,33 @@
         <v>0.26</v>
       </c>
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="n">
         <v>0.24</v>
       </c>
       <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -848,16 +839,16 @@
         <v>0.14</v>
       </c>
       <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15">
@@ -868,13 +859,13 @@
         <v>0.14</v>
       </c>
       <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -888,16 +879,16 @@
         <v>0.1</v>
       </c>
       <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>54</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17">
@@ -908,16 +899,16 @@
         <v>0.08</v>
       </c>
       <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>58</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>59</v>
-      </c>
-      <c r="F17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18">
@@ -928,16 +919,16 @@
         <v>0.06</v>
       </c>
       <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>62</v>
       </c>
-      <c r="E18" t="s">
-        <v>63</v>
-      </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19">
@@ -948,16 +939,16 @@
         <v>0.06</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
@@ -965,19 +956,19 @@
         <v>6</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21">
@@ -988,13 +979,13 @@
         <v>-0.13</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -1008,16 +999,16 @@
         <v>-0.13</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23">
@@ -1028,56 +1019,56 @@
         <v>-0.76</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="n">
         <v>-0.84</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="n">
         <v>-0.85</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26">
@@ -1088,13 +1079,13 @@
         <v>-0.86</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -1108,16 +1099,16 @@
         <v>-0.86</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28">
@@ -1128,16 +1119,16 @@
         <v>-0.87</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
@@ -1148,16 +1139,16 @@
         <v>-0.87</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>